<commit_message>
implement the react frontend
</commit_message>
<xml_diff>
--- a/backend/Users.xlsx
+++ b/backend/Users.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -407,7 +407,7 @@
         <v>sdfsdf</v>
       </c>
       <c r="B1" t="str">
-        <v>sdfsdf</v>
+        <v>sdfsdf_1</v>
       </c>
       <c r="C1" t="str">
         <v>sdfsdf@dfsdfsdf.com</v>
@@ -417,45 +417,60 @@
       </c>
       <c r="E1" t="str">
         <v>AgACAgIAAxkBAAPxZ-GliwIU-pKwdFmjlDQuFjegcgEAApL9MRuP_QlLLl2QDn_tu7ABAAMCAAN3AAM2BA</v>
+      </c>
+      <c r="F1" t="str">
+        <v>chatId</v>
+      </c>
+      <c r="G1" t="str">
+        <v>firstName</v>
+      </c>
+      <c r="H1" t="str">
+        <v>lastName</v>
+      </c>
+      <c r="I1" t="str">
+        <v>email</v>
+      </c>
+      <c r="J1" t="str">
+        <v>imageUrl</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Moin</v>
+        <v>Huntrick</v>
       </c>
       <c r="B2" t="str">
-        <v>Looser</v>
+        <v>GB</v>
       </c>
       <c r="C2" t="str">
-        <v>looser@gmail.com</v>
+        <v>huntrick@gmail.com</v>
       </c>
       <c r="D2" t="str">
         <v>USDT</v>
       </c>
       <c r="E2" t="str">
-        <v>AgACAgIAAxkBAAPxZ-GliwIU-pKwdFmjlDQuFjegcgEAApL9MRuP_QlLLl2QDn_tu7ABAAMCAAN3AAM2BA</v>
+        <v>AgACAgIAAxkBAAIBiWfhtJaGFGUSa8oyqUl4J5uzqNwaAAJT7jEbnVMIS1hpkXQDSbihAQADAgADeAADNgQ</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
-        <v>Huntrick</v>
-      </c>
-      <c r="B3" t="str">
-        <v>GB</v>
-      </c>
-      <c r="C3" t="str">
-        <v>huntrick@gmail.com</v>
-      </c>
-      <c r="D3" t="str">
-        <v>USDT</v>
-      </c>
-      <c r="E3" t="str">
-        <v>AgACAgIAAxkBAAIBiWfhtJaGFGUSa8oyqUl4J5uzqNwaAAJT7jEbnVMIS1hpkXQDSbihAQADAgADeAADNgQ</v>
+      <c r="F3">
+        <v>5038824563</v>
+      </c>
+      <c r="G3" t="str">
+        <v>sadfasdf</v>
+      </c>
+      <c r="H3" t="str">
+        <v>dfasdfsad</v>
+      </c>
+      <c r="I3" t="str">
+        <v>asdfasdf@sdfasdf.com</v>
+      </c>
+      <c r="J3" t="str">
+        <v>https://api.telegram.org/file/bot7203212788:AAF46vpGtp-c0vGf8Twd3flL4tFSFvZKMXM/photos/file_0.jpg</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>